<commit_message>
Updating Futures and FRA Excel workbooks
</commit_message>
<xml_diff>
--- a/03 Products & Pricing/FRAs.xlsx
+++ b/03 Products & Pricing/FRAs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\BOOK\.SWAPS_BOOK\03 Products &amp; Pricing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6068D556-473E-462C-9A0F-DA2B14B92C75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96AFFFED-A8E6-42F3-BCB8-0084CF15BD84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{25739176-8D93-4B8D-A4B5-B1CE389BD96E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{25739176-8D93-4B8D-A4B5-B1CE389BD96E}"/>
   </bookViews>
   <sheets>
     <sheet name="FRA Quotes" sheetId="1" r:id="rId1"/>
@@ -4746,7 +4746,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAF093D6-E372-413F-BAB0-B4C68DA83186}">
   <dimension ref="B2:E17"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -5305,14 +5305,14 @@
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="N19:O19"/>
+    <mergeCell ref="R20:S20"/>
+    <mergeCell ref="N20:O20"/>
     <mergeCell ref="J23:M23"/>
     <mergeCell ref="L19:M19"/>
     <mergeCell ref="B19:C19"/>
     <mergeCell ref="F19:G19"/>
     <mergeCell ref="H19:I19"/>
-    <mergeCell ref="N19:O19"/>
-    <mergeCell ref="R20:S20"/>
-    <mergeCell ref="N20:O20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5323,7 +5323,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{772DF092-E2C4-4B8D-A9A0-C641D736BFF6}">
   <dimension ref="B2:M23"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>